<commit_message>
Correct the handling of non-string column names if the column name is None
</commit_message>
<xml_diff>
--- a/examples/test_numeric_column_name.xlsx
+++ b/examples/test_numeric_column_name.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Sites/shared/pulls/agate-excel/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,12 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Country</t>
   </si>
   <si>
     <t>Canada</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
 </sst>
 </file>
@@ -347,13 +350,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -361,12 +364,15 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>35160000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>